<commit_message>
Prev word check + predicat with prev verb.
</commit_message>
<xml_diff>
--- a/prepositions.xlsx
+++ b/prepositions.xlsx
@@ -114,19 +114,16 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="204"/>
       <family val="0"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="204"/>
       <family val="0"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="204"/>
       <family val="0"/>
       <sz val="10"/>
     </font>
@@ -157,7 +154,7 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium"/>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
   </borders>
@@ -190,7 +187,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -211,12 +208,11 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F9" activeCellId="0" pane="topLeft" sqref="F9"/>
+      <selection activeCell="D6" activeCellId="0" pane="topLeft" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.73725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="1">
@@ -334,7 +330,7 @@
       <c r="C6" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="3" t="n">
         <v>17</v>
       </c>
       <c r="E6" s="3" t="n">
@@ -681,9 +677,8 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.73725490196078"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -707,9 +702,8 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.73725490196078"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>